<commit_message>
Updated data form format.
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3704D3FA-2810-4151-9E1E-19DE3719CA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5319D7-DAF1-423E-B7FE-3B5C2429AA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-12045" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Stop</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>FileName</t>
+  </si>
+  <si>
+    <t>да</t>
   </si>
 </sst>
 </file>
@@ -433,12 +436,13 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
@@ -526,6 +530,10 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3" t="str">
+        <f>F3</f>
+        <v>Сидоров Сидор Сидорович</v>
+      </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
@@ -564,8 +572,12 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B6" si="0">F4</f>
+        <v>Коинов Герберт Боитович</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -605,6 +617,10 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Машинина Маша Мишина</v>
+      </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
@@ -644,6 +660,10 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>Поидов Николай Сайгакович</v>
+      </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>

</xml_diff>